<commit_message>
Commit with updates of ACE 017 in the log
</commit_message>
<xml_diff>
--- a/Derek's Log.xlsx
+++ b/Derek's Log.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="150" windowWidth="14865" windowHeight="10785" tabRatio="440"/>
   </bookViews>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
   <si>
     <t>Staff Name</t>
   </si>
@@ -353,9 +348,6 @@
     <t>106</t>
   </si>
   <si>
-    <t>Built in PC. No demo required. Log in for external client.</t>
-  </si>
-  <si>
     <t>1530</t>
   </si>
   <si>
@@ -368,13 +360,60 @@
     <t>S203</t>
   </si>
   <si>
-    <t>Shut down PC and ceiling projector. N203 key</t>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
+    <t>1900</t>
+  </si>
+  <si>
+    <t>S205</t>
+  </si>
+  <si>
+    <t>157A</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <r>
+      <t>Door code</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 11012*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>No demo required. Log in for external client.</t>
+  </si>
+  <si>
+    <t>N203 key</t>
+  </si>
+  <si>
+    <t>Pickup VHS cart and connecting cables. N203 key</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -417,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,6 +477,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,7 +540,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -538,6 +583,39 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -550,9 +628,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -601,7 +676,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -634,26 +709,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -686,23 +744,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -882,10 +923,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +941,7 @@
     <col min="7" max="16384" width="22.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
@@ -919,64 +961,150 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="10">
-        <v>42571</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B3" s="10">
+        <v>42570</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="10">
-        <v>42571</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>110</v>
-      </c>
       <c r="F3" s="19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B4" s="10">
-        <v>42571</v>
+        <v>42570</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>61</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="10">
+        <v>42570</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="26">
+        <v>42571</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>113</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="26">
+        <v>42571</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="26">
+        <v>42571</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -985,12 +1113,15 @@
     <sortCondition ref="C427:C515"/>
     <sortCondition ref="D427:D515"/>
   </sortState>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5 B6 B2 A7:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D1048576 E6 E2 D3:D5">
       <formula1>Building</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2">
+      <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tested with todays data
</commit_message>
<xml_diff>
--- a/Derek's Log.xlsx
+++ b/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="139">
   <si>
     <t>Staff Name</t>
   </si>
@@ -406,6 +406,62 @@
   </si>
   <si>
     <t>305 SCR</t>
+  </si>
+  <si>
+    <t>MONDAY</t>
+  </si>
+  <si>
+    <t>Pickup VHS cart and connecting cables. N203 key.</t>
+  </si>
+  <si>
+    <t>157A</t>
+  </si>
+  <si>
+    <r>
+      <t>Door code</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 11012*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>1700</t>
+  </si>
+  <si>
+    <t>1022</t>
+  </si>
+  <si>
+    <t>Class moved here from Ross S102. Not on RAC report</t>
+  </si>
+  <si>
+    <t>1630</t>
+  </si>
+  <si>
+    <t>McLaughlin</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>Drawer does not lock.</t>
   </si>
 </sst>
 </file>
@@ -538,7 +594,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -611,6 +667,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -918,11 +977,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,7 +989,7 @@
     <col min="1" max="1" width="27.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="19" style="10" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="9" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="11" customWidth="1"/>
     <col min="6" max="6" width="60.42578125" style="19" customWidth="1"/>
     <col min="7" max="16384" width="22.140625" style="3"/>
@@ -1235,6 +1294,152 @@
         <v>125</v>
       </c>
     </row>
+    <row r="17" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+    </row>
+    <row r="18" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="26">
+        <v>42576</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="26">
+        <v>42576</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="26">
+        <v>42576</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="10">
+        <v>42577</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="10">
+        <v>42577</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="10">
+        <v>42577</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">
@@ -1242,13 +1447,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5 B6 B2 A7:A8 B9 A10:A16 A17:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A26:A1048576 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A22:A24 A3:A5">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D3:D5 D7:D8 E9 D10:D16 D17:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D26:D1048576 D7:D8 E9 D10:D16 E17 D18:D20 E21 D22:D24 D3:D5">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>